<commit_message>
chore: 完成 product 相关修改
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/template-RMB.xlsx
+++ b/src/main/resources/templates/excel/template-RMB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rick/Space/Workspace/product-manager/src/main/resources/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F48E5C-90BB-B548-8C38-E3376A45672F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5473F294-5BBE-4F48-A9FC-CBA217DB0CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="760" windowWidth="33060" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="173">
   <si>
     <t>Tel:  +86 187 6196 5038  Office Tel: +86 0512 6763 4077  Fax: +86 0512 6763 4077</t>
   </si>
@@ -666,30 +666,30 @@
   </si>
   <si>
     <t>Packing information:</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>RM203,2F,No.214 Kuachun Road, Suzhou industrial park, Jiangsu, 215121 China</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Remarks:</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>1. Sample order payment term: 100% upon order confirmation</t>
   </si>
   <si>
     <t xml:space="preserve">Production lead time: </t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Suzhou Compass Machinery &amp; Electric Co., Ltd</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Optional functions and extra cost</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Quotation</t>
@@ -700,24 +700,15 @@
   <si>
     <t>MOQ
 (pcs)</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Certificates:</t>
-    <phoneticPr fontId="31" type="noConversion"/>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Quotation No.:</t>
-    <phoneticPr fontId="31" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Company: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whats App: </t>
+    <phoneticPr fontId="30" type="noConversion"/>
   </si>
   <si>
     <t>Unit Price
@@ -734,18 +725,38 @@
     <t>EXW</t>
   </si>
   <si>
-    <t xml:space="preserve">Contact: </t>
+    <t xml:space="preserve">MOQ: </t>
+  </si>
+  <si>
+    <t>¥</t>
+  </si>
+  <si>
+    <t>进价</t>
+  </si>
+  <si>
+    <t>税</t>
+  </si>
+  <si>
+    <t>利润率</t>
+  </si>
+  <si>
+    <t>汇率</t>
+  </si>
+  <si>
+    <t>报价</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;¥&quot;#,##0.00;[Red]&quot;¥&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;¥&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="39">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -897,14 +908,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
@@ -973,40 +976,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1038,8 +1007,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1055,18 +1039,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1320,7 +1292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1469,36 +1441,15 @@
     <xf numFmtId="1" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1508,10 +1459,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1541,26 +1492,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="40" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1574,19 +1507,19 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1595,40 +1528,28 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1646,7 +1567,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1655,22 +1576,22 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="35" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="35" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1682,13 +1603,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="42" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="36" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="8" fontId="40" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1697,13 +1618,13 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="42" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1712,22 +1633,22 @@
     <xf numFmtId="1" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="40" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="8" fontId="40" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="41" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="35" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="41" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="35" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1756,6 +1677,45 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1850,15 +1810,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>441675</xdr:colOff>
+      <xdr:colOff>451835</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>138997</xdr:rowOff>
+      <xdr:rowOff>169477</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>721360</xdr:colOff>
+      <xdr:colOff>700755</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>159738</xdr:rowOff>
+      <xdr:rowOff>164397</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1887,8 +1847,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6781515" y="13357157"/>
-          <a:ext cx="1427765" cy="1422821"/>
+          <a:off x="6791675" y="13387637"/>
+          <a:ext cx="1397000" cy="1397000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2161,494 +2121,519 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="125" zoomScaleNormal="95" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.1640625" style="50" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" style="50" customWidth="1"/>
     <col min="3" max="3" width="39.1640625" style="50" customWidth="1"/>
-    <col min="4" max="6" width="15" style="68" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="101" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="78" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="78" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="78" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="50" customWidth="1"/>
+    <col min="4" max="6" width="15" style="61" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="132" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="132" customWidth="1"/>
+    <col min="9" max="9" width="10" style="132" customWidth="1"/>
+    <col min="10" max="10" width="8" style="132" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="132" customWidth="1"/>
     <col min="12" max="12" width="7.5" style="50"/>
     <col min="13" max="13" width="8.83203125" style="50" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="7.5" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" customHeight="1">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
     </row>
     <row r="2" spans="1:11" ht="14" customHeight="1">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="123" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="77"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:11" ht="14" customHeight="1">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="77"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
     </row>
     <row r="4" spans="1:11" ht="30.5" customHeight="1">
-      <c r="A4" s="142" t="s">
+      <c r="A4" s="125" t="s">
         <v>157</v>
       </c>
-      <c r="B4" s="142"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="77"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="I4" s="131"/>
     </row>
     <row r="5" spans="1:11" ht="16.25" customHeight="1">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="95"/>
+      <c r="F5" s="90"/>
+    </row>
+    <row r="6" spans="1:11" ht="17.75" customHeight="1">
+      <c r="A6" s="110"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="95"/>
+      <c r="F6" s="90"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.75" customHeight="1">
+      <c r="A7" s="93"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="96" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="90"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.25" customHeight="1">
+      <c r="A8" s="110"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.25" customHeight="1">
+      <c r="A9" s="87"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="K9" s="132" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="48" customFormat="1" ht="66.5" customHeight="1">
+      <c r="A10" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="108" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" s="112"/>
-      <c r="F5" s="107"/>
-    </row>
-    <row r="6" spans="1:11" ht="17.75" customHeight="1">
-      <c r="A6" s="127" t="s">
+      <c r="F10" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="108" t="s">
+      <c r="G10" s="132" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="132" t="s">
+        <v>169</v>
+      </c>
+      <c r="I10" s="132" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" s="132" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" s="132" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="49" customFormat="1" ht="409" customHeight="1">
+      <c r="A11" s="115">
         <v>1</v>
       </c>
-      <c r="E6" s="112"/>
-      <c r="F6" s="107"/>
-    </row>
-    <row r="7" spans="1:11" ht="17.75" customHeight="1">
-      <c r="A7" s="110" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="108" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="113" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="107"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.25" customHeight="1">
-      <c r="A8" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.25" customHeight="1">
-      <c r="A9" s="104"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-    </row>
-    <row r="10" spans="1:11" s="48" customFormat="1" ht="66.5" customHeight="1">
-      <c r="A10" s="96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="96" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="111" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="97" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="97" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="101"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="56"/>
-    </row>
-    <row r="11" spans="1:11" s="49" customFormat="1" ht="409" customHeight="1">
-      <c r="A11" s="132">
-        <v>1</v>
-      </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136">
+      <c r="B11" s="116"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119">
         <f>D11*E11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="100"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="58"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="134">
+        <v>1</v>
+      </c>
+      <c r="I11" s="135">
+        <v>1</v>
+      </c>
+      <c r="J11" s="135"/>
+      <c r="K11" s="136">
+        <f>IF(AND(G9="¥",K9="$"),G11/I11/J11/H11,IF(AND(G9="$",K9="¥"),G11/I11*J11, G11/I11/H11))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="49" customFormat="1" ht="52" customHeight="1">
-      <c r="A12" s="132"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="135"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="136"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="58"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="136"/>
     </row>
     <row r="13" spans="1:11" s="49" customFormat="1" ht="38.5" customHeight="1">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="120" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="58"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="132"/>
+      <c r="J13" s="132"/>
+      <c r="K13" s="132"/>
     </row>
     <row r="14" spans="1:11" s="49" customFormat="1" ht="84" customHeight="1">
       <c r="A14" s="51"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125">
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108">
         <f t="shared" ref="F14" si="0">D14*E14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="100"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="53"/>
+      <c r="G14" s="137"/>
+      <c r="H14" s="137">
+        <v>1</v>
+      </c>
+      <c r="I14" s="138">
+        <v>1</v>
+      </c>
+      <c r="J14" s="138"/>
+      <c r="K14" s="139">
+        <f>IF(AND(G12="¥",K12="$"),G14/I14/J14/H14,IF(AND(G12="$",K12="¥"),G14/I14*J14, G14/I14/H14))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="49" customFormat="1" ht="35" customHeight="1">
-      <c r="A15" s="128" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="124">
+      <c r="A15" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="107">
         <f>SUM(E11:E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="124">
+      <c r="F15" s="107">
         <f>SUM(F11:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="102"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="57"/>
+      <c r="G15" s="140"/>
+      <c r="H15" s="140"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="132"/>
+      <c r="K15" s="132"/>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="87" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="D16" s="89" t="s">
+      <c r="D16" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="E16" s="90"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="141"/>
+      <c r="J16" s="141"/>
     </row>
     <row r="17" spans="1:12" ht="22.75" customHeight="1">
-      <c r="A17" s="59"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="130"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1">
-      <c r="A18" s="59"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="123" t="s">
+      <c r="A18" s="54"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="106" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="100"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
+      <c r="J18" s="141"/>
+    </row>
+    <row r="19" spans="1:12" ht="20.5" customHeight="1">
+      <c r="A19" s="54"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="141"/>
+    </row>
+    <row r="20" spans="1:12" ht="18" customHeight="1">
+      <c r="A20" s="54"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="D18" s="117"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-    </row>
-    <row r="19" spans="1:12" ht="20.5" customHeight="1">
-      <c r="A19" s="59"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-    </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1">
-      <c r="A20" s="59"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="71"/>
-      <c r="I20" s="80"/>
-      <c r="K20" s="52"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="64"/>
+      <c r="J20" s="141"/>
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1">
-      <c r="A21" s="59"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="119"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="82"/>
-      <c r="K21" s="52"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="142"/>
+      <c r="J21" s="143"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1">
-      <c r="A22" s="59"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="61"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="141"/>
+      <c r="J22" s="141"/>
+      <c r="K22" s="141"/>
     </row>
     <row r="23" spans="1:12" ht="20.5" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="119"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="61"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141"/>
     </row>
     <row r="24" spans="1:12" ht="18" customHeight="1">
-      <c r="A24" s="59"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="61"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="141"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="141"/>
+      <c r="J24" s="141"/>
+      <c r="K24" s="141"/>
     </row>
     <row r="25" spans="1:12" ht="18" customHeight="1">
-      <c r="A25" s="59"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="60"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="141"/>
+      <c r="H25" s="141"/>
+      <c r="I25" s="141"/>
+      <c r="J25" s="141"/>
+      <c r="K25" s="141"/>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1">
-      <c r="A26" s="64"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="70"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="63"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="63"/>
+      <c r="I26" s="142"/>
+      <c r="J26" s="143"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="56"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1">
       <c r="A27"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="94"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="63"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="143"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="56"/>
     </row>
     <row r="28" spans="1:12" ht="18" customHeight="1">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="62"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="55"/>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1">
-      <c r="A29" s="85" t="s">
+      <c r="A29" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="85"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="74"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="62"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="67"/>
+      <c r="I29" s="141"/>
+      <c r="J29" s="141"/>
+      <c r="K29" s="141"/>
+      <c r="L29" s="55"/>
     </row>
     <row r="30" spans="1:12" ht="18" customHeight="1">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="74"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="62"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="I30" s="141"/>
+      <c r="J30" s="141"/>
+      <c r="K30" s="141"/>
+      <c r="L30" s="55"/>
     </row>
     <row r="31" spans="1:12" ht="18" customHeight="1">
-      <c r="A31" s="98"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="62"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="I31" s="141"/>
+      <c r="J31" s="141"/>
+      <c r="K31" s="141"/>
+      <c r="L31" s="55"/>
     </row>
     <row r="32" spans="1:12" ht="18" customHeight="1">
-      <c r="B32" s="99"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="74"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="62"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="I32" s="141"/>
+      <c r="J32" s="141"/>
+      <c r="K32" s="141"/>
+      <c r="L32" s="55"/>
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1">
-      <c r="A33" s="131" t="s">
+      <c r="A33" s="114" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="131"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="83"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="70"/>
     </row>
     <row r="34" spans="1:6" ht="18" customHeight="1">
       <c r="A34" s="49"/>
       <c r="B34" s="49"/>
       <c r="C34" s="49"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1">
       <c r="A35" s="49"/>
       <c r="B35" s="49"/>
       <c r="C35" s="49"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
     </row>
     <row r="36" spans="1:6" ht="18" customHeight="1">
       <c r="A36" s="49"/>
       <c r="B36" s="49"/>
       <c r="C36" s="49"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="18" customHeight="1">
       <c r="A37" s="49"/>
       <c r="B37" s="49"/>
       <c r="C37" s="49"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="19">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
@@ -2664,7 +2649,7 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A13:D13"/>
   </mergeCells>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.64" right="0.35" top="0.23622047244094491" bottom="0.15748031496062992" header="0.19685039370078741" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -3288,28 +3273,28 @@
       <c r="A27" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="143">
+      <c r="B27" s="126">
         <v>345</v>
       </c>
-      <c r="C27" s="144"/>
-      <c r="D27" s="144"/>
-      <c r="E27" s="144"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="145"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
+      <c r="G27" s="128"/>
     </row>
     <row r="28" spans="1:7" ht="25.25" hidden="1" customHeight="1">
       <c r="A28" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="143">
+      <c r="B28" s="126">
         <f>SUMPRODUCT(B25:G25,B26:G26)+B27</f>
         <v>9815</v>
       </c>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="128"/>
     </row>
     <row r="29" spans="1:7" ht="25.25" customHeight="1">
       <c r="A29" s="46"/>
@@ -3326,15 +3311,15 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.25" hidden="1" customHeight="1">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="146"/>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="129"/>
     </row>
     <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="26" t="s">
@@ -3347,15 +3332,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="52.25" hidden="1" customHeight="1">
-      <c r="A34" s="147" t="s">
+      <c r="A34" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="147"/>
-      <c r="C34" s="147"/>
-      <c r="D34" s="147"/>
-      <c r="E34" s="147"/>
-      <c r="F34" s="147"/>
-      <c r="G34" s="147"/>
+      <c r="B34" s="130"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="130"/>
+      <c r="E34" s="130"/>
+      <c r="F34" s="130"/>
+      <c r="G34" s="130"/>
     </row>
     <row r="35" spans="1:7" hidden="1"/>
   </sheetData>
@@ -3365,7 +3350,7 @@
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="A34:G34"/>
   </mergeCells>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -4747,7 +4732,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="30" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>